<commit_message>
Update: Edit the content of ANN algorithm comparison
</commit_message>
<xml_diff>
--- a/Documents/BaoCaoGiuaKy/Bang_dang_gia_thuat_toan.xlsx
+++ b/Documents/BaoCaoGiuaKy/Bang_dang_gia_thuat_toan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\BaoCaoGiuaKy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\KLTN-WeatherForecast\Documents\BaoCaoGiuaKy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B47822-44EB-4267-B76D-EFB599C791AB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD21841-52BA-4CAF-B5D5-1622CB579DB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{5D9979D5-C377-417E-9506-A7702014EB99}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Algorithm</t>
   </si>
@@ -76,6 +76,53 @@
     <t>- Easy to apply in solution
 - Fast execution
 - Perceptron compability</t>
+  </si>
+  <si>
+    <t>- Not work with non-linear data types
+- Require independent data points</t>
+  </si>
+  <si>
+    <t>- Training complexity is 0
+- Prediction is simple</t>
+  </si>
+  <si>
+    <t>- With small K, KNN is very sensitive
+- Cost a lot of time for calculation, especially with big database</t>
+  </si>
+  <si>
+    <t>- Be able to solve classification problems with classes</t>
+  </si>
+  <si>
+    <t>- Only compatiple with data which class is near linearly separable</t>
+  </si>
+  <si>
+    <t>- Unlimited data whether it's linear or not
+- Boundary depends on training data
+- Expandable</t>
+  </si>
+  <si>
+    <t>- Discrete data can cause problems
+- Take time to analyze models</t>
+  </si>
+  <si>
+    <t>- Not require to identify models neuron, fuzy logic, ...
+- Good for multi-dimension problems
+- Well handle overfitting</t>
+  </si>
+  <si>
+    <t>- High complexity
+- Limitations on processing numeric data
+- Probability is not clearly deminstrated</t>
+  </si>
+  <si>
+    <t>- Reasonable training time
+- Fast application
+- Easy to interpret
+- Easy to implement</t>
+  </si>
+  <si>
+    <t>- Cannot handle complicated relationship
+- Simple decision boundaries</t>
   </si>
 </sst>
 </file>
@@ -86,7 +133,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -139,25 +186,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,90 +519,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4B8142-C51B-4056-A579-60F210F01743}">
   <dimension ref="B2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="35.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="4"/>
+    <col min="2" max="2" width="28.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.75" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>